<commit_message>
Update MS4 Traceability Matrix Report
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestsDocuments/ms4-traceability-matrix-group5.xlsx
+++ b/Documents/Testing/TestsDocuments/ms4-traceability-matrix-group5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicole Chan\Desktop\Seneca-Summer-2023\SFT221\Milestone Project\MS4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA983E33-8DB5-43FB-B1D2-C3DC979BBAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F9ECDE-A24B-45E8-91E4-0E3AB7892294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="125">
   <si>
     <t xml:space="preserve">Requirements </t>
   </si>
@@ -126,9 +126,6 @@
   </si>
   <si>
     <t>ABC123</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
   <si>
     <t>T018</t>
@@ -649,9 +646,6 @@
     <t>1A</t>
   </si>
   <si>
-    <t>22Y</t>
-  </si>
-  <si>
     <t>225U</t>
   </si>
   <si>
@@ -676,22 +670,63 @@
     <t>(Cannot Exit)</t>
   </si>
   <si>
-    <t>R003 - MS4 Version ii</t>
-  </si>
-  <si>
-    <t>R002 - MS4 Version i</t>
+    <t>R003</t>
+  </si>
+  <si>
+    <t>R002 - MS4</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>T043</t>
+  </si>
+  <si>
+    <t>T044</t>
+  </si>
+  <si>
+    <t>T045</t>
+  </si>
+  <si>
+    <t>T046</t>
+  </si>
+  <si>
+    <t>T047</t>
+  </si>
+  <si>
+    <t>24Y</t>
+  </si>
+  <si>
+    <t>T048</t>
+  </si>
+  <si>
+    <t>23Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -768,13 +803,6 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -877,74 +905,107 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -952,30 +1013,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1253,15 +1290,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M63"/>
+  <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J2"/>
+    <sheetView tabSelected="1" topLeftCell="D42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.21875" style="21" customWidth="1"/>
+    <col min="1" max="1" width="26.21875" style="16" customWidth="1"/>
     <col min="2" max="2" width="9" style="1" customWidth="1"/>
     <col min="3" max="3" width="35.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="36" style="1" customWidth="1"/>
@@ -1269,11 +1306,11 @@
     <col min="6" max="6" width="45.44140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="41.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.77734375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="41.33203125" style="21" customWidth="1"/>
-    <col min="10" max="10" width="15.77734375" style="21" customWidth="1"/>
-    <col min="11" max="11" width="41.33203125" style="21" customWidth="1"/>
-    <col min="12" max="12" width="15.77734375" style="21" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="21"/>
+    <col min="9" max="9" width="41.33203125" style="16" customWidth="1"/>
+    <col min="10" max="10" width="15.77734375" style="16" customWidth="1"/>
+    <col min="11" max="11" width="41.33203125" style="16" customWidth="1"/>
+    <col min="12" max="12" width="15.77734375" style="16" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1">
@@ -1289,18 +1326,18 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="L2" s="18"/>
+      <c r="G2" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" s="31"/>
+      <c r="I2" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" s="31"/>
+      <c r="K2" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="L2" s="31"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickBot="1">
@@ -1320,23 +1357,23 @@
       <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="I3" s="19" t="s">
+      <c r="H3" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="K3" s="19" t="s">
+      <c r="J3" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="20" t="s">
-        <v>69</v>
+      <c r="L3" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="M3" s="4"/>
     </row>
@@ -1344,11 +1381,11 @@
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>42</v>
+      <c r="C4" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>41</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -1359,22 +1396,22 @@
       <c r="G4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H4" s="31" t="s">
-        <v>79</v>
+      <c r="H4" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="I4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="J4" s="31" t="s">
-        <v>79</v>
+      <c r="J4" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="32"/>
       <c r="E5" s="1">
         <v>1000</v>
       </c>
@@ -1384,22 +1421,22 @@
       <c r="G5" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H5" s="31" t="s">
-        <v>79</v>
+      <c r="H5" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="I5" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="J5" s="31" t="s">
-        <v>79</v>
+      <c r="J5" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="32"/>
       <c r="E6" s="1">
         <v>-0.1</v>
       </c>
@@ -1409,22 +1446,22 @@
       <c r="G6" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H6" s="31" t="s">
-        <v>79</v>
+      <c r="H6" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="I6" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="J6" s="31" t="s">
-        <v>79</v>
+      <c r="J6" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="32"/>
       <c r="E7" s="1">
         <v>1000.1</v>
       </c>
@@ -1434,26 +1471,26 @@
       <c r="G7" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H7" s="31" t="s">
-        <v>79</v>
+      <c r="H7" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="I7" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="J7" s="31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" s="26" customFormat="1"/>
+      <c r="J7" s="23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="33" customFormat="1"/>
     <row r="9" spans="1:13" ht="43.2" customHeight="1">
       <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>43</v>
+      <c r="C9" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>42</v>
       </c>
       <c r="E9" s="1">
         <v>0.25</v>
@@ -1464,22 +1501,22 @@
       <c r="G9" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H9" s="31" t="s">
-        <v>79</v>
+      <c r="H9" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="I9" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="J9" s="31" t="s">
-        <v>79</v>
+      <c r="J9" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="32"/>
       <c r="E10" s="1">
         <v>0.5</v>
       </c>
@@ -1489,22 +1526,22 @@
       <c r="G10" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H10" s="31" t="s">
-        <v>79</v>
+      <c r="H10" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="I10" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="J10" s="31" t="s">
-        <v>79</v>
+      <c r="J10" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="32"/>
       <c r="E11" s="1">
         <v>1</v>
       </c>
@@ -1514,22 +1551,22 @@
       <c r="G11" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H11" s="31" t="s">
-        <v>79</v>
+      <c r="H11" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="I11" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="J11" s="31" t="s">
-        <v>79</v>
+      <c r="J11" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="32"/>
       <c r="E12" s="1">
         <v>0.24</v>
       </c>
@@ -1539,22 +1576,22 @@
       <c r="G12" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H12" s="31" t="s">
-        <v>79</v>
+      <c r="H12" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="I12" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="J12" s="31" t="s">
-        <v>79</v>
+      <c r="J12" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="B13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="32"/>
       <c r="E13" s="1">
         <v>-0.5</v>
       </c>
@@ -1564,22 +1601,22 @@
       <c r="G13" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H13" s="31" t="s">
-        <v>79</v>
+      <c r="H13" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="I13" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="J13" s="31" t="s">
-        <v>79</v>
+      <c r="J13" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="B14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="32"/>
       <c r="E14" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -1589,26 +1626,26 @@
       <c r="G14" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H14" s="31" t="s">
-        <v>79</v>
+      <c r="H14" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="I14" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="J14" s="31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" s="26" customFormat="1"/>
+      <c r="J14" s="23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="33" customFormat="1"/>
     <row r="16" spans="1:13">
       <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>44</v>
+      <c r="C16" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>43</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>25</v>
@@ -1619,22 +1656,22 @@
       <c r="G16" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H16" s="31" t="s">
-        <v>79</v>
+      <c r="H16" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="I16" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="J16" s="31" t="s">
-        <v>79</v>
+      <c r="J16" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="2:10">
       <c r="B17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
       <c r="E17" s="1" t="s">
         <v>26</v>
       </c>
@@ -1644,124 +1681,124 @@
       <c r="G17" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="H17" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="I17" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J17" s="31" t="s">
-        <v>79</v>
+      <c r="H17" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="I17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="2:10">
       <c r="B18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
       <c r="E18" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F18" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G18" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="I18" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="J18" s="31" t="s">
-        <v>79</v>
+      <c r="G18" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="I18" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="2:10">
       <c r="B19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
       <c r="E19" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F19" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G19" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="I19" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19" s="31" t="s">
-        <v>79</v>
+      <c r="G19" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="I19" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="2:10">
       <c r="B20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
       <c r="E20" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F20" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G20" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="I20" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="J20" s="31" t="s">
-        <v>79</v>
+      <c r="G20" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="I20" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="2:10">
       <c r="B21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
       <c r="E21" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F21" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G21" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H21" s="22" t="s">
-        <v>78</v>
+      <c r="G21" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>77</v>
       </c>
       <c r="I21" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="J21" s="31" t="s">
-        <v>79</v>
+        <v>0</v>
+      </c>
+      <c r="J21" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="2:10">
       <c r="B22" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
       <c r="E22" s="1" t="s">
-        <v>31</v>
+        <v>116</v>
       </c>
       <c r="F22" s="1" t="b">
         <v>1</v>
@@ -1769,74 +1806,74 @@
       <c r="G22" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="H22" s="22" t="s">
-        <v>78</v>
+      <c r="H22" s="17" t="s">
+        <v>77</v>
       </c>
       <c r="I22" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="J22" s="22" t="s">
-        <v>78</v>
+      <c r="J22" s="17" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="2:10">
       <c r="B23" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
+        <v>31</v>
+      </c>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
       <c r="E23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F23" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G23" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="I23" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="J23" s="31" t="s">
-        <v>79</v>
+      <c r="G23" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="I23" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="2:10">
       <c r="B24" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
+        <v>32</v>
+      </c>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
       <c r="E24" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F24" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G24" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H24" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="H24" s="22" t="s">
-        <v>78</v>
-      </c>
       <c r="I24" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="J24" s="17" t="s">
         <v>77</v>
-      </c>
-      <c r="J24" s="22" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="25" spans="2:10">
       <c r="B25" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
+        <v>35</v>
+      </c>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
       <c r="E25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F25" s="1" t="b">
         <v>0</v>
@@ -1844,341 +1881,341 @@
       <c r="G25" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H25" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="I25" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J25" s="31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" s="26" customFormat="1"/>
+      <c r="H25" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="I25" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J25" s="23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" s="33" customFormat="1"/>
     <row r="27" spans="2:10" ht="28.8" customHeight="1">
       <c r="B27" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="F27" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="H27" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="J27" s="22" t="s">
-        <v>78</v>
+        <v>80</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="I27" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="J27" s="17" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="2:10">
       <c r="B28" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="16"/>
+        <v>38</v>
+      </c>
+      <c r="C28" s="29"/>
+      <c r="D28" s="32"/>
       <c r="E28" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H28" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="I28" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="J28" s="22" t="s">
-        <v>78</v>
+        <v>82</v>
+      </c>
+      <c r="H28" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="I28" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="J28" s="17" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="2:10">
       <c r="B29" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="16"/>
+        <v>39</v>
+      </c>
+      <c r="C29" s="29"/>
+      <c r="D29" s="32"/>
       <c r="E29" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H29" s="31" t="s">
-        <v>79</v>
+        <v>83</v>
+      </c>
+      <c r="H29" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="J29" s="31" t="s">
-        <v>79</v>
+        <v>83</v>
+      </c>
+      <c r="J29" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="2:10">
       <c r="B30" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="16"/>
+        <v>40</v>
+      </c>
+      <c r="C30" s="29"/>
+      <c r="D30" s="32"/>
       <c r="E30" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H30" s="31" t="s">
-        <v>79</v>
+        <v>84</v>
+      </c>
+      <c r="H30" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="J30" s="31" t="s">
-        <v>79</v>
+        <v>84</v>
+      </c>
+      <c r="J30" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="2:10">
       <c r="B31" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="16"/>
+        <v>49</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="32"/>
       <c r="E31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="G31" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H31" s="31" t="s">
-        <v>79</v>
+        <v>82</v>
+      </c>
+      <c r="H31" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J31" s="31" t="s">
-        <v>79</v>
+        <v>82</v>
+      </c>
+      <c r="J31" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="2:10">
       <c r="B32" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="16"/>
+        <v>50</v>
+      </c>
+      <c r="C32" s="29"/>
+      <c r="D32" s="32"/>
       <c r="E32" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H32" s="31" t="s">
-        <v>79</v>
+        <v>83</v>
+      </c>
+      <c r="H32" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="J32" s="31" t="s">
-        <v>79</v>
+        <v>83</v>
+      </c>
+      <c r="J32" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="2:10">
       <c r="B33" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="16"/>
+        <v>51</v>
+      </c>
+      <c r="C33" s="29"/>
+      <c r="D33" s="32"/>
       <c r="E33" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H33" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="I33" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="J33" s="31" t="s">
-        <v>79</v>
+        <v>85</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="I33" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="J33" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="2:10">
       <c r="B34" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="16"/>
+        <v>60</v>
+      </c>
+      <c r="C34" s="29"/>
+      <c r="D34" s="32"/>
       <c r="E34" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H34" s="31" t="s">
-        <v>79</v>
+        <v>83</v>
+      </c>
+      <c r="H34" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="J34" s="31" t="s">
-        <v>79</v>
+        <v>83</v>
+      </c>
+      <c r="J34" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="2:10">
       <c r="B35" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="16"/>
+        <v>61</v>
+      </c>
+      <c r="C35" s="29"/>
+      <c r="D35" s="32"/>
       <c r="E35" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H35" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="I35" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="J35" s="31" t="s">
-        <v>79</v>
+        <v>85</v>
+      </c>
+      <c r="H35" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="I35" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="J35" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="2:10">
       <c r="B36" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="16"/>
+        <v>64</v>
+      </c>
+      <c r="C36" s="29"/>
+      <c r="D36" s="32"/>
       <c r="E36" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H36" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="I36" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="J36" s="31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" s="26" customFormat="1"/>
+        <v>85</v>
+      </c>
+      <c r="H36" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="I36" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="J36" s="23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" s="33" customFormat="1"/>
     <row r="38" spans="2:10" ht="43.2">
       <c r="B38" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F38" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="E38" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>73</v>
-      </c>
       <c r="G38" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="H38" s="31" t="s">
-        <v>79</v>
+        <v>72</v>
+      </c>
+      <c r="H38" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="J38" s="31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" s="26" customFormat="1"/>
+        <v>72</v>
+      </c>
+      <c r="J38" s="23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" s="33" customFormat="1"/>
     <row r="40" spans="2:10">
       <c r="B40" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="F40" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="G40" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="H40" s="31" t="s">
+      <c r="E40" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="I40" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="J40" s="22" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" s="26" customFormat="1"/>
+      <c r="F40" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="H40" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="I40" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="J40" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" s="33" customFormat="1"/>
     <row r="42" spans="2:10" ht="14.4" customHeight="1">
       <c r="B42" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C42" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>44</v>
+        <v>86</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="D42" s="32" t="s">
+        <v>43</v>
       </c>
       <c r="E42" s="1">
         <v>34.353999999999999</v>
@@ -2186,137 +2223,137 @@
       <c r="F42" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G42" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H42" s="24" t="s">
-        <v>111</v>
+      <c r="G42" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H42" s="18" t="s">
+        <v>109</v>
       </c>
       <c r="I42" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="J42" s="31" t="s">
-        <v>79</v>
+      <c r="J42" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="2:10">
       <c r="B43" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" s="23"/>
-      <c r="D43" s="16"/>
+        <v>87</v>
+      </c>
+      <c r="C43" s="27"/>
+      <c r="D43" s="32"/>
       <c r="E43" s="1">
         <v>1</v>
       </c>
       <c r="F43" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G43" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H43" s="24" t="s">
-        <v>111</v>
+      <c r="G43" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H43" s="18" t="s">
+        <v>109</v>
       </c>
       <c r="I43" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="J43" s="31" t="s">
-        <v>79</v>
+      <c r="J43" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="2:10">
       <c r="B44" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C44" s="23"/>
-      <c r="D44" s="16"/>
+        <v>88</v>
+      </c>
+      <c r="C44" s="27"/>
+      <c r="D44" s="32"/>
       <c r="E44" s="1">
         <v>1000</v>
       </c>
       <c r="F44" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G44" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H44" s="24" t="s">
-        <v>111</v>
+      <c r="G44" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H44" s="18" t="s">
+        <v>109</v>
       </c>
       <c r="I44" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="J44" s="31" t="s">
-        <v>79</v>
+      <c r="J44" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="2:10">
       <c r="B45" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C45" s="23"/>
-      <c r="D45" s="16"/>
+        <v>89</v>
+      </c>
+      <c r="C45" s="27"/>
+      <c r="D45" s="32"/>
       <c r="E45" s="1">
         <v>1234.3209999999999</v>
       </c>
       <c r="F45" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G45" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H45" s="24" t="s">
-        <v>111</v>
+      <c r="G45" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H45" s="18" t="s">
+        <v>109</v>
       </c>
       <c r="I45" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="J45" s="31" t="s">
-        <v>79</v>
+      <c r="J45" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="2:10">
       <c r="B46" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C46" s="23"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="24" t="s">
-        <v>103</v>
+        <v>90</v>
+      </c>
+      <c r="C46" s="27"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="F46" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G46" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H46" s="24" t="s">
-        <v>111</v>
+      <c r="G46" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>109</v>
       </c>
       <c r="I46" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="J46" s="22" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" s="27" customFormat="1">
-      <c r="B47" s="28"/>
-      <c r="E47" s="28"/>
-      <c r="F47" s="28"/>
-      <c r="G47" s="29"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="28"/>
-      <c r="J47" s="28"/>
+      <c r="J46" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" s="20" customFormat="1">
+      <c r="B47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="19"/>
     </row>
     <row r="48" spans="2:10" ht="14.4" customHeight="1">
       <c r="B48" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C48" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="D48" s="16" t="s">
-        <v>43</v>
+        <v>91</v>
+      </c>
+      <c r="C48" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="D48" s="32" t="s">
+        <v>42</v>
       </c>
       <c r="E48" s="1">
         <v>0.25</v>
@@ -2324,297 +2361,322 @@
       <c r="F48" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G48" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H48" s="24" t="s">
-        <v>111</v>
+      <c r="G48" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H48" s="18" t="s">
+        <v>109</v>
       </c>
       <c r="I48" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="J48" s="31" t="s">
-        <v>79</v>
+      <c r="J48" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="2:10">
       <c r="B49" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C49" s="15"/>
-      <c r="D49" s="16"/>
+        <v>92</v>
+      </c>
+      <c r="C49" s="29"/>
+      <c r="D49" s="32"/>
       <c r="E49" s="1">
         <v>0.5</v>
       </c>
       <c r="F49" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G49" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H49" s="24" t="s">
-        <v>111</v>
+      <c r="G49" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H49" s="18" t="s">
+        <v>109</v>
       </c>
       <c r="I49" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="J49" s="31" t="s">
-        <v>79</v>
+      <c r="J49" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="2:10">
       <c r="B50" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="16"/>
+        <v>93</v>
+      </c>
+      <c r="C50" s="29"/>
+      <c r="D50" s="32"/>
       <c r="E50" s="1">
         <v>1</v>
       </c>
       <c r="F50" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G50" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H50" s="24" t="s">
-        <v>111</v>
+      <c r="G50" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H50" s="18" t="s">
+        <v>109</v>
       </c>
       <c r="I50" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="J50" s="31" t="s">
-        <v>79</v>
+      <c r="J50" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="2:10">
       <c r="B51" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C51" s="15"/>
-      <c r="D51" s="16"/>
+        <v>94</v>
+      </c>
+      <c r="C51" s="29"/>
+      <c r="D51" s="32"/>
       <c r="E51" s="1">
         <v>0.75</v>
       </c>
       <c r="F51" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G51" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H51" s="24" t="s">
-        <v>111</v>
+      <c r="G51" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H51" s="18" t="s">
+        <v>109</v>
       </c>
       <c r="I51" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="J51" s="31" t="s">
-        <v>79</v>
+      <c r="J51" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="2:10">
       <c r="B52" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C52" s="15"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="24" t="s">
-        <v>104</v>
+        <v>95</v>
+      </c>
+      <c r="C52" s="29"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="18" t="s">
+        <v>103</v>
       </c>
       <c r="F52" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G52" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H52" s="24" t="s">
-        <v>111</v>
+      <c r="G52" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H52" s="18" t="s">
+        <v>109</v>
       </c>
       <c r="I52" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="J52" s="31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="53" spans="2:10" s="26" customFormat="1"/>
+      <c r="J52" s="23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" s="33" customFormat="1"/>
     <row r="54" spans="2:10" ht="14.4" customHeight="1">
       <c r="B54" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C54" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="D54" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E54" s="24" t="s">
-        <v>105</v>
+        <v>117</v>
+      </c>
+      <c r="C54" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="D54" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="E54" s="18" t="s">
+        <v>104</v>
       </c>
       <c r="F54" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G54" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H54" s="24" t="s">
-        <v>111</v>
+      <c r="G54" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H54" s="18" t="s">
+        <v>109</v>
       </c>
       <c r="I54" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="J54" s="31" t="s">
-        <v>79</v>
+      <c r="J54" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="2:10">
       <c r="B55" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C55" s="23"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="24" t="s">
-        <v>106</v>
+        <v>118</v>
+      </c>
+      <c r="C55" s="27"/>
+      <c r="D55" s="32"/>
+      <c r="E55" s="18" t="s">
+        <v>105</v>
       </c>
       <c r="F55" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G55" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H55" s="24" t="s">
-        <v>111</v>
+      <c r="G55" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H55" s="18" t="s">
+        <v>109</v>
       </c>
       <c r="I55" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="J55" s="22" t="s">
-        <v>78</v>
+      <c r="J55" s="17" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="2:10">
       <c r="B56" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C56" s="23"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="24" t="s">
-        <v>107</v>
+        <v>119</v>
+      </c>
+      <c r="C56" s="27"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="35" t="s">
+        <v>122</v>
       </c>
       <c r="F56" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G56" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H56" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="I56" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="J56" s="30" t="s">
-        <v>112</v>
+      <c r="G56" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H56" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="I56" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J56" s="17" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="2:10">
       <c r="B57" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C57" s="23"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="24" t="s">
-        <v>108</v>
+        <v>120</v>
+      </c>
+      <c r="C57" s="27"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="35" t="s">
+        <v>124</v>
       </c>
       <c r="F57" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G57" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H57" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="I57" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J57" s="31" t="s">
-        <v>79</v>
+        <v>1</v>
+      </c>
+      <c r="G57" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="H57" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="I57" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="J57" s="22" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="2:10">
       <c r="B58" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C58" s="23"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="24" t="s">
-        <v>109</v>
+        <v>121</v>
+      </c>
+      <c r="C58" s="27"/>
+      <c r="D58" s="32"/>
+      <c r="E58" s="18" t="s">
+        <v>106</v>
       </c>
       <c r="F58" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G58" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H58" s="24" t="s">
-        <v>111</v>
+      <c r="G58" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>109</v>
       </c>
       <c r="I58" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="J58" s="31" t="s">
-        <v>79</v>
+      <c r="J58" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="2:10">
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
+      <c r="B59" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C59" s="27"/>
+      <c r="D59" s="32"/>
+      <c r="E59" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="F59" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G59" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H59" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="I59" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J59" s="23" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="60" spans="2:10">
-      <c r="C60" s="21"/>
-      <c r="D60" s="21"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
     </row>
     <row r="61" spans="2:10">
-      <c r="C61" s="21"/>
-      <c r="D61" s="21"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="16"/>
     </row>
     <row r="62" spans="2:10">
-      <c r="C62" s="21"/>
-      <c r="D62" s="21"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
     </row>
     <row r="63" spans="2:10">
-      <c r="C63" s="21"/>
-      <c r="D63" s="21"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+    </row>
+    <row r="64" spans="2:10">
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="24">
     <mergeCell ref="C48:C52"/>
     <mergeCell ref="D48:D52"/>
-    <mergeCell ref="C54:C58"/>
-    <mergeCell ref="D54:D58"/>
+    <mergeCell ref="C54:C59"/>
+    <mergeCell ref="D54:D59"/>
     <mergeCell ref="A53:XFD53"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
     <mergeCell ref="C42:C46"/>
     <mergeCell ref="D42:D46"/>
     <mergeCell ref="A39:XFD39"/>
     <mergeCell ref="A26:XFD26"/>
     <mergeCell ref="A15:XFD15"/>
-    <mergeCell ref="A8:XFD8"/>
     <mergeCell ref="A37:XFD37"/>
     <mergeCell ref="A41:XFD41"/>
-    <mergeCell ref="K2:L2"/>
     <mergeCell ref="C27:C36"/>
     <mergeCell ref="D27:D36"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="D9:D14"/>
     <mergeCell ref="D16:D25"/>
     <mergeCell ref="C16:C25"/>
     <mergeCell ref="C9:C14"/>
     <mergeCell ref="C4:C7"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="A8:XFD8"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="D9:D14"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E36" r:id="rId1" xr:uid="{06DC9311-2D25-46B2-8DF2-1A11B71FA734}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Updated Test Descriptions and Matrix for MS4
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestsDocuments/ms4-traceability-matrix-group5.xlsx
+++ b/Documents/Testing/TestsDocuments/ms4-traceability-matrix-group5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicole Chan\Desktop\Seneca-Summer-2023\SFT221\Milestone Project\MS4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F9ECDE-A24B-45E8-91E4-0E3AB7892294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC45908-1810-4221-8775-83867AAF992F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="126">
   <si>
     <t xml:space="preserve">Requirements </t>
   </si>
@@ -582,7 +582,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Validation for DESTINATION input</t>
+Validation for package SIZE input</t>
     </r>
   </si>
   <si>
@@ -602,12 +602,86 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Validation for package SIZE input</t>
-    </r>
+Validation for DESTINATION input</t>
+    </r>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>5F</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>225U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$#%2345sdsa </t>
+  </si>
+  <si>
+    <t>R001 - MS3</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>NOT RUN</t>
+  </si>
+  <si>
+    <t>(No message shown)</t>
+  </si>
+  <si>
+    <t>Input failed</t>
+  </si>
+  <si>
+    <t>(Cannot Exit)</t>
+  </si>
+  <si>
+    <t>R003</t>
+  </si>
+  <si>
+    <t>R002 - MS4</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>T043</t>
+  </si>
+  <si>
+    <t>T044</t>
+  </si>
+  <si>
+    <t>T045</t>
+  </si>
+  <si>
+    <t>T046</t>
+  </si>
+  <si>
+    <t>T047</t>
+  </si>
+  <si>
+    <t>24Y</t>
+  </si>
+  <si>
+    <t>T048</t>
+  </si>
+  <si>
+    <t>23Y</t>
+  </si>
+  <si>
+    <t>Linking the function validatePackageWeight() to unit test and
+use assert (AreEqual) for testing. 
+If the expected result matches the actual results, test case pass.</t>
   </si>
   <si>
     <r>
@@ -626,93 +700,31 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Validation for DESTINATION input</t>
-    </r>
-  </si>
-  <si>
-    <t>$</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>5F</t>
-  </si>
-  <si>
-    <t>1A</t>
-  </si>
-  <si>
-    <t>225U</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$#%2345sdsa </t>
-  </si>
-  <si>
-    <t>R001 - MS3</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>NOT RUN</t>
-  </si>
-  <si>
-    <t>(No message shown)</t>
-  </si>
-  <si>
-    <t>Input failed</t>
-  </si>
-  <si>
-    <t>(Cannot Exit)</t>
-  </si>
-  <si>
-    <t>R003</t>
-  </si>
-  <si>
-    <t>R002 - MS4</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>T043</t>
-  </si>
-  <si>
-    <t>T044</t>
-  </si>
-  <si>
-    <t>T045</t>
-  </si>
-  <si>
-    <t>T046</t>
-  </si>
-  <si>
-    <t>T047</t>
-  </si>
-  <si>
-    <t>24Y</t>
-  </si>
-  <si>
-    <t>T048</t>
-  </si>
-  <si>
-    <t>23Y</t>
+Validation for package WEIGHT input</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -905,29 +917,29 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -936,83 +948,86 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1292,8 +1307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42:C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1326,18 +1341,18 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="J2" s="31"/>
-      <c r="K2" s="30" t="s">
+      <c r="G2" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2" s="35"/>
+      <c r="I2" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="L2" s="31"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="L2" s="35"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickBot="1">
@@ -1381,10 +1396,10 @@
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="36" t="s">
         <v>41</v>
       </c>
       <c r="E4" s="1">
@@ -1411,7 +1426,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="29"/>
-      <c r="D5" s="32"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="1">
         <v>1000</v>
       </c>
@@ -1436,7 +1451,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="29"/>
-      <c r="D6" s="32"/>
+      <c r="D6" s="30"/>
       <c r="E6" s="1">
         <v>-0.1</v>
       </c>
@@ -1461,7 +1476,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="29"/>
-      <c r="D7" s="32"/>
+      <c r="D7" s="30"/>
       <c r="E7" s="1">
         <v>1000.1</v>
       </c>
@@ -1481,15 +1496,15 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="33" customFormat="1"/>
+    <row r="8" spans="1:13" s="32" customFormat="1"/>
     <row r="9" spans="1:13" ht="43.2" customHeight="1">
       <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="36" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="1">
@@ -1516,7 +1531,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="29"/>
-      <c r="D10" s="32"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="1">
         <v>0.5</v>
       </c>
@@ -1541,7 +1556,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="29"/>
-      <c r="D11" s="32"/>
+      <c r="D11" s="30"/>
       <c r="E11" s="1">
         <v>1</v>
       </c>
@@ -1566,7 +1581,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="29"/>
-      <c r="D12" s="32"/>
+      <c r="D12" s="30"/>
       <c r="E12" s="1">
         <v>0.24</v>
       </c>
@@ -1591,7 +1606,7 @@
         <v>16</v>
       </c>
       <c r="C13" s="29"/>
-      <c r="D13" s="32"/>
+      <c r="D13" s="30"/>
       <c r="E13" s="1">
         <v>-0.5</v>
       </c>
@@ -1616,7 +1631,7 @@
         <v>17</v>
       </c>
       <c r="C14" s="29"/>
-      <c r="D14" s="32"/>
+      <c r="D14" s="30"/>
       <c r="E14" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -1636,15 +1651,15 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="33" customFormat="1"/>
+    <row r="15" spans="1:13" s="32" customFormat="1"/>
     <row r="16" spans="1:13">
       <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="D16" s="32" t="s">
+      <c r="D16" s="30" t="s">
         <v>43</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -1670,8 +1685,8 @@
       <c r="B17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
       <c r="E17" s="1" t="s">
         <v>26</v>
       </c>
@@ -1695,8 +1710,8 @@
       <c r="B18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
       <c r="E18" s="1" t="s">
         <v>27</v>
       </c>
@@ -1720,8 +1735,8 @@
       <c r="B19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
       <c r="E19" s="1" t="s">
         <v>28</v>
       </c>
@@ -1745,8 +1760,8 @@
       <c r="B20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
       <c r="E20" s="1" t="s">
         <v>29</v>
       </c>
@@ -1770,8 +1785,8 @@
       <c r="B21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
       <c r="E21" s="1" t="s">
         <v>30</v>
       </c>
@@ -1795,10 +1810,10 @@
       <c r="B22" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
       <c r="E22" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F22" s="1" t="b">
         <v>1</v>
@@ -1820,8 +1835,8 @@
       <c r="B23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
       <c r="E23" s="1" t="s">
         <v>33</v>
       </c>
@@ -1845,8 +1860,8 @@
       <c r="B24" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
       <c r="E24" s="1" t="s">
         <v>34</v>
       </c>
@@ -1870,8 +1885,8 @@
       <c r="B25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
       <c r="E25" s="1" t="s">
         <v>37</v>
       </c>
@@ -1891,15 +1906,15 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="2:10" s="33" customFormat="1"/>
+    <row r="26" spans="2:10" s="32" customFormat="1"/>
     <row r="27" spans="2:10" ht="28.8" customHeight="1">
       <c r="B27" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="32" t="s">
+      <c r="D27" s="36" t="s">
         <v>44</v>
       </c>
       <c r="E27" s="1" t="s">
@@ -1926,7 +1941,7 @@
         <v>38</v>
       </c>
       <c r="C28" s="29"/>
-      <c r="D28" s="32"/>
+      <c r="D28" s="30"/>
       <c r="E28" s="1" t="s">
         <v>46</v>
       </c>
@@ -1940,7 +1955,7 @@
         <v>77</v>
       </c>
       <c r="I28" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J28" s="17" t="s">
         <v>77</v>
@@ -1951,7 +1966,7 @@
         <v>39</v>
       </c>
       <c r="C29" s="29"/>
-      <c r="D29" s="32"/>
+      <c r="D29" s="30"/>
       <c r="E29" s="1" t="s">
         <v>47</v>
       </c>
@@ -1976,7 +1991,7 @@
         <v>40</v>
       </c>
       <c r="C30" s="29"/>
-      <c r="D30" s="32"/>
+      <c r="D30" s="30"/>
       <c r="E30" s="1" t="s">
         <v>48</v>
       </c>
@@ -2001,7 +2016,7 @@
         <v>49</v>
       </c>
       <c r="C31" s="29"/>
-      <c r="D31" s="32"/>
+      <c r="D31" s="30"/>
       <c r="E31" s="1" t="s">
         <v>55</v>
       </c>
@@ -2026,7 +2041,7 @@
         <v>50</v>
       </c>
       <c r="C32" s="29"/>
-      <c r="D32" s="32"/>
+      <c r="D32" s="30"/>
       <c r="E32" s="6" t="s">
         <v>59</v>
       </c>
@@ -2051,7 +2066,7 @@
         <v>51</v>
       </c>
       <c r="C33" s="29"/>
-      <c r="D33" s="32"/>
+      <c r="D33" s="30"/>
       <c r="E33" s="1" t="s">
         <v>65</v>
       </c>
@@ -2065,7 +2080,7 @@
         <v>77</v>
       </c>
       <c r="I33" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J33" s="23" t="s">
         <v>78</v>
@@ -2076,7 +2091,7 @@
         <v>60</v>
       </c>
       <c r="C34" s="29"/>
-      <c r="D34" s="32"/>
+      <c r="D34" s="30"/>
       <c r="E34" s="1" t="s">
         <v>62</v>
       </c>
@@ -2101,7 +2116,7 @@
         <v>61</v>
       </c>
       <c r="C35" s="29"/>
-      <c r="D35" s="32"/>
+      <c r="D35" s="30"/>
       <c r="E35" s="1" t="s">
         <v>63</v>
       </c>
@@ -2115,7 +2130,7 @@
         <v>77</v>
       </c>
       <c r="I35" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J35" s="23" t="s">
         <v>78</v>
@@ -2126,7 +2141,7 @@
         <v>64</v>
       </c>
       <c r="C36" s="29"/>
-      <c r="D36" s="32"/>
+      <c r="D36" s="30"/>
       <c r="E36" s="7" t="s">
         <v>66</v>
       </c>
@@ -2140,13 +2155,13 @@
         <v>77</v>
       </c>
       <c r="I36" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J36" s="23" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="2:10" s="33" customFormat="1"/>
+    <row r="37" spans="2:10" s="32" customFormat="1"/>
     <row r="38" spans="2:10" ht="43.2">
       <c r="B38" s="4" t="s">
         <v>69</v>
@@ -2176,7 +2191,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="2:10" s="33" customFormat="1"/>
+    <row r="39" spans="2:10" s="32" customFormat="1"/>
     <row r="40" spans="2:10">
       <c r="B40" s="4" t="s">
         <v>73</v>
@@ -2200,22 +2215,22 @@
         <v>78</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J40" s="17" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="2:10" s="33" customFormat="1"/>
+    <row r="41" spans="2:10" s="32" customFormat="1"/>
     <row r="42" spans="2:10" ht="14.4" customHeight="1">
       <c r="B42" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C42" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="D42" s="32" t="s">
-        <v>43</v>
+      <c r="C42" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="D42" s="36" t="s">
+        <v>124</v>
       </c>
       <c r="E42" s="1">
         <v>34.353999999999999</v>
@@ -2224,10 +2239,10 @@
         <v>1</v>
       </c>
       <c r="G42" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H42" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I42" s="1" t="b">
         <v>1</v>
@@ -2240,8 +2255,8 @@
       <c r="B43" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="27"/>
-      <c r="D43" s="32"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="30"/>
       <c r="E43" s="1">
         <v>1</v>
       </c>
@@ -2249,10 +2264,10 @@
         <v>1</v>
       </c>
       <c r="G43" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H43" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I43" s="1" t="b">
         <v>1</v>
@@ -2265,8 +2280,8 @@
       <c r="B44" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C44" s="27"/>
-      <c r="D44" s="32"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="30"/>
       <c r="E44" s="1">
         <v>1000</v>
       </c>
@@ -2274,10 +2289,10 @@
         <v>1</v>
       </c>
       <c r="G44" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H44" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I44" s="1" t="b">
         <v>1</v>
@@ -2290,8 +2305,8 @@
       <c r="B45" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C45" s="27"/>
-      <c r="D45" s="32"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="30"/>
       <c r="E45" s="1">
         <v>1234.3209999999999</v>
       </c>
@@ -2299,10 +2314,10 @@
         <v>0</v>
       </c>
       <c r="G45" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H45" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I45" s="1" t="b">
         <v>0</v>
@@ -2315,19 +2330,19 @@
       <c r="B46" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="27"/>
-      <c r="D46" s="32"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="30"/>
       <c r="E46" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F46" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G46" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H46" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I46" s="1" t="b">
         <v>1</v>
@@ -2349,10 +2364,10 @@
       <c r="B48" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C48" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="D48" s="32" t="s">
+      <c r="C48" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="D48" s="30" t="s">
         <v>42</v>
       </c>
       <c r="E48" s="1">
@@ -2362,10 +2377,10 @@
         <v>1</v>
       </c>
       <c r="G48" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H48" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I48" s="1" t="b">
         <v>1</v>
@@ -2379,7 +2394,7 @@
         <v>92</v>
       </c>
       <c r="C49" s="29"/>
-      <c r="D49" s="32"/>
+      <c r="D49" s="30"/>
       <c r="E49" s="1">
         <v>0.5</v>
       </c>
@@ -2387,10 +2402,10 @@
         <v>1</v>
       </c>
       <c r="G49" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H49" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I49" s="1" t="b">
         <v>1</v>
@@ -2404,7 +2419,7 @@
         <v>93</v>
       </c>
       <c r="C50" s="29"/>
-      <c r="D50" s="32"/>
+      <c r="D50" s="30"/>
       <c r="E50" s="1">
         <v>1</v>
       </c>
@@ -2412,10 +2427,10 @@
         <v>1</v>
       </c>
       <c r="G50" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H50" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I50" s="1" t="b">
         <v>1</v>
@@ -2429,7 +2444,7 @@
         <v>94</v>
       </c>
       <c r="C51" s="29"/>
-      <c r="D51" s="32"/>
+      <c r="D51" s="30"/>
       <c r="E51" s="1">
         <v>0.75</v>
       </c>
@@ -2437,10 +2452,10 @@
         <v>0</v>
       </c>
       <c r="G51" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H51" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I51" s="1" t="b">
         <v>0</v>
@@ -2454,18 +2469,18 @@
         <v>95</v>
       </c>
       <c r="C52" s="29"/>
-      <c r="D52" s="32"/>
+      <c r="D52" s="30"/>
       <c r="E52" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F52" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G52" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H52" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I52" s="1" t="b">
         <v>0</v>
@@ -2474,28 +2489,28 @@
         <v>78</v>
       </c>
     </row>
-    <row r="53" spans="2:10" s="33" customFormat="1"/>
+    <row r="53" spans="2:10" s="32" customFormat="1"/>
     <row r="54" spans="2:10" ht="14.4" customHeight="1">
       <c r="B54" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C54" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="D54" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="C54" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="D54" s="31" t="s">
         <v>43</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F54" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G54" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H54" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I54" s="1" t="b">
         <v>1</v>
@@ -2506,21 +2521,21 @@
     </row>
     <row r="55" spans="2:10">
       <c r="B55" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="C55" s="27"/>
-      <c r="D55" s="32"/>
+        <v>117</v>
+      </c>
+      <c r="C55" s="28"/>
+      <c r="D55" s="30"/>
       <c r="E55" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F55" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G55" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H55" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I55" s="1" t="b">
         <v>1</v>
@@ -2531,21 +2546,21 @@
     </row>
     <row r="56" spans="2:10">
       <c r="B56" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C56" s="27"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="35" t="s">
-        <v>122</v>
+        <v>118</v>
+      </c>
+      <c r="C56" s="28"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="27" t="s">
+        <v>121</v>
       </c>
       <c r="F56" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G56" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H56" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I56" s="1" t="b">
         <v>0</v>
@@ -2556,46 +2571,46 @@
     </row>
     <row r="57" spans="2:10">
       <c r="B57" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="C57" s="27"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="35" t="s">
-        <v>124</v>
+        <v>119</v>
+      </c>
+      <c r="C57" s="28"/>
+      <c r="D57" s="30"/>
+      <c r="E57" s="27" t="s">
+        <v>123</v>
       </c>
       <c r="F57" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G57" s="35" t="s">
+      <c r="G57" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="H57" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="I57" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="H57" s="35" t="s">
+      <c r="J57" s="22" t="s">
         <v>109</v>
-      </c>
-      <c r="I57" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="J57" s="22" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="58" spans="2:10">
       <c r="B58" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="C58" s="27"/>
-      <c r="D58" s="32"/>
+        <v>120</v>
+      </c>
+      <c r="C58" s="28"/>
+      <c r="D58" s="30"/>
       <c r="E58" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F58" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G58" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H58" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I58" s="1" t="b">
         <v>0</v>
@@ -2606,21 +2621,21 @@
     </row>
     <row r="59" spans="2:10">
       <c r="B59" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="C59" s="27"/>
-      <c r="D59" s="32"/>
+        <v>122</v>
+      </c>
+      <c r="C59" s="28"/>
+      <c r="D59" s="30"/>
       <c r="E59" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F59" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G59" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H59" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I59" s="1" t="b">
         <v>0</v>
@@ -2651,11 +2666,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C48:C52"/>
-    <mergeCell ref="D48:D52"/>
-    <mergeCell ref="C54:C59"/>
-    <mergeCell ref="D54:D59"/>
-    <mergeCell ref="A53:XFD53"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="A8:XFD8"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="D9:D14"/>
     <mergeCell ref="C42:C46"/>
     <mergeCell ref="D42:D46"/>
     <mergeCell ref="A39:XFD39"/>
@@ -2667,16 +2685,13 @@
     <mergeCell ref="D27:D36"/>
     <mergeCell ref="D16:D25"/>
     <mergeCell ref="C16:C25"/>
-    <mergeCell ref="C9:C14"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="A8:XFD8"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="D9:D14"/>
+    <mergeCell ref="C48:C52"/>
+    <mergeCell ref="D48:D52"/>
+    <mergeCell ref="C54:C59"/>
+    <mergeCell ref="D54:D59"/>
+    <mergeCell ref="A53:XFD53"/>
   </mergeCells>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E36" r:id="rId1" xr:uid="{06DC9311-2D25-46B2-8DF2-1A11B71FA734}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Updated Matrix for MS4
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestsDocuments/ms4-traceability-matrix-group5.xlsx
+++ b/Documents/Testing/TestsDocuments/ms4-traceability-matrix-group5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicole Chan\Desktop\Seneca-Summer-2023\SFT221\Milestone Project\MS4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC45908-1810-4221-8775-83867AAF992F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44413887-DC7A-4871-97D9-D3BFD7131813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -679,11 +679,6 @@
     <t>23Y</t>
   </si>
   <si>
-    <t>Linking the function validatePackageWeight() to unit test and
-use assert (AreEqual) for testing. 
-If the expected result matches the actual results, test case pass.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -707,17 +702,52 @@
 Validation for package WEIGHT input</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Linking the function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>validatePackageWeight()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to unit test and
+use assert (AreEqual) for testing. 
+If the expected result matches the actual results, test case pass.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -917,29 +947,29 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -948,85 +978,85 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1307,8 +1337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42:C46"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1316,7 +1346,7 @@
     <col min="1" max="1" width="26.21875" style="16" customWidth="1"/>
     <col min="2" max="2" width="9" style="1" customWidth="1"/>
     <col min="3" max="3" width="35.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="36" style="1" customWidth="1"/>
+    <col min="4" max="4" width="39.21875" style="1" customWidth="1"/>
     <col min="5" max="5" width="23.21875" style="1" customWidth="1"/>
     <col min="6" max="6" width="45.44140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="41.33203125" style="1" customWidth="1"/>
@@ -1341,18 +1371,18 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="H2" s="35"/>
-      <c r="I2" s="34" t="s">
+      <c r="H2" s="31"/>
+      <c r="I2" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="J2" s="35"/>
-      <c r="K2" s="34" t="s">
+      <c r="J2" s="31"/>
+      <c r="K2" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="L2" s="35"/>
+      <c r="L2" s="31"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickBot="1">
@@ -1396,10 +1426,10 @@
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="28" t="s">
         <v>41</v>
       </c>
       <c r="E4" s="1">
@@ -1426,7 +1456,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="29"/>
-      <c r="D5" s="30"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="1">
         <v>1000</v>
       </c>
@@ -1451,7 +1481,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="29"/>
-      <c r="D6" s="30"/>
+      <c r="D6" s="33"/>
       <c r="E6" s="1">
         <v>-0.1</v>
       </c>
@@ -1476,7 +1506,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="29"/>
-      <c r="D7" s="30"/>
+      <c r="D7" s="33"/>
       <c r="E7" s="1">
         <v>1000.1</v>
       </c>
@@ -1501,10 +1531,10 @@
       <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="28" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="1">
@@ -1531,7 +1561,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="29"/>
-      <c r="D10" s="30"/>
+      <c r="D10" s="33"/>
       <c r="E10" s="1">
         <v>0.5</v>
       </c>
@@ -1556,7 +1586,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="29"/>
-      <c r="D11" s="30"/>
+      <c r="D11" s="33"/>
       <c r="E11" s="1">
         <v>1</v>
       </c>
@@ -1581,7 +1611,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="29"/>
-      <c r="D12" s="30"/>
+      <c r="D12" s="33"/>
       <c r="E12" s="1">
         <v>0.24</v>
       </c>
@@ -1606,7 +1636,7 @@
         <v>16</v>
       </c>
       <c r="C13" s="29"/>
-      <c r="D13" s="30"/>
+      <c r="D13" s="33"/>
       <c r="E13" s="1">
         <v>-0.5</v>
       </c>
@@ -1631,7 +1661,7 @@
         <v>17</v>
       </c>
       <c r="C14" s="29"/>
-      <c r="D14" s="30"/>
+      <c r="D14" s="33"/>
       <c r="E14" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -1656,10 +1686,10 @@
       <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="33" t="s">
         <v>43</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -1685,8 +1715,8 @@
       <c r="B17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
       <c r="E17" s="1" t="s">
         <v>26</v>
       </c>
@@ -1710,8 +1740,8 @@
       <c r="B18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
       <c r="E18" s="1" t="s">
         <v>27</v>
       </c>
@@ -1735,8 +1765,8 @@
       <c r="B19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
       <c r="E19" s="1" t="s">
         <v>28</v>
       </c>
@@ -1760,8 +1790,8 @@
       <c r="B20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
       <c r="E20" s="1" t="s">
         <v>29</v>
       </c>
@@ -1785,8 +1815,8 @@
       <c r="B21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
       <c r="E21" s="1" t="s">
         <v>30</v>
       </c>
@@ -1810,8 +1840,8 @@
       <c r="B22" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
       <c r="E22" s="1" t="s">
         <v>115</v>
       </c>
@@ -1835,8 +1865,8 @@
       <c r="B23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
       <c r="E23" s="1" t="s">
         <v>33</v>
       </c>
@@ -1860,8 +1890,8 @@
       <c r="B24" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
       <c r="E24" s="1" t="s">
         <v>34</v>
       </c>
@@ -1885,8 +1915,8 @@
       <c r="B25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
       <c r="E25" s="1" t="s">
         <v>37</v>
       </c>
@@ -1911,10 +1941,10 @@
       <c r="B27" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="36" t="s">
+      <c r="D27" s="28" t="s">
         <v>44</v>
       </c>
       <c r="E27" s="1" t="s">
@@ -1941,7 +1971,7 @@
         <v>38</v>
       </c>
       <c r="C28" s="29"/>
-      <c r="D28" s="30"/>
+      <c r="D28" s="33"/>
       <c r="E28" s="1" t="s">
         <v>46</v>
       </c>
@@ -1966,7 +1996,7 @@
         <v>39</v>
       </c>
       <c r="C29" s="29"/>
-      <c r="D29" s="30"/>
+      <c r="D29" s="33"/>
       <c r="E29" s="1" t="s">
         <v>47</v>
       </c>
@@ -1991,7 +2021,7 @@
         <v>40</v>
       </c>
       <c r="C30" s="29"/>
-      <c r="D30" s="30"/>
+      <c r="D30" s="33"/>
       <c r="E30" s="1" t="s">
         <v>48</v>
       </c>
@@ -2016,7 +2046,7 @@
         <v>49</v>
       </c>
       <c r="C31" s="29"/>
-      <c r="D31" s="30"/>
+      <c r="D31" s="33"/>
       <c r="E31" s="1" t="s">
         <v>55</v>
       </c>
@@ -2041,7 +2071,7 @@
         <v>50</v>
       </c>
       <c r="C32" s="29"/>
-      <c r="D32" s="30"/>
+      <c r="D32" s="33"/>
       <c r="E32" s="6" t="s">
         <v>59</v>
       </c>
@@ -2066,7 +2096,7 @@
         <v>51</v>
       </c>
       <c r="C33" s="29"/>
-      <c r="D33" s="30"/>
+      <c r="D33" s="33"/>
       <c r="E33" s="1" t="s">
         <v>65</v>
       </c>
@@ -2091,7 +2121,7 @@
         <v>60</v>
       </c>
       <c r="C34" s="29"/>
-      <c r="D34" s="30"/>
+      <c r="D34" s="33"/>
       <c r="E34" s="1" t="s">
         <v>62</v>
       </c>
@@ -2116,7 +2146,7 @@
         <v>61</v>
       </c>
       <c r="C35" s="29"/>
-      <c r="D35" s="30"/>
+      <c r="D35" s="33"/>
       <c r="E35" s="1" t="s">
         <v>63</v>
       </c>
@@ -2141,7 +2171,7 @@
         <v>64</v>
       </c>
       <c r="C36" s="29"/>
-      <c r="D36" s="30"/>
+      <c r="D36" s="33"/>
       <c r="E36" s="7" t="s">
         <v>66</v>
       </c>
@@ -2226,11 +2256,11 @@
       <c r="B42" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C42" s="36" t="s">
+      <c r="C42" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="D42" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="D42" s="36" t="s">
-        <v>124</v>
       </c>
       <c r="E42" s="1">
         <v>34.353999999999999</v>
@@ -2255,8 +2285,8 @@
       <c r="B43" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="28"/>
-      <c r="D43" s="30"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="33"/>
       <c r="E43" s="1">
         <v>1</v>
       </c>
@@ -2280,8 +2310,8 @@
       <c r="B44" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C44" s="28"/>
-      <c r="D44" s="30"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="33"/>
       <c r="E44" s="1">
         <v>1000</v>
       </c>
@@ -2305,8 +2335,8 @@
       <c r="B45" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C45" s="28"/>
-      <c r="D45" s="30"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="33"/>
       <c r="E45" s="1">
         <v>1234.3209999999999</v>
       </c>
@@ -2330,8 +2360,8 @@
       <c r="B46" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="30"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="33"/>
       <c r="E46" s="18" t="s">
         <v>101</v>
       </c>
@@ -2364,10 +2394,10 @@
       <c r="B48" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C48" s="28" t="s">
+      <c r="C48" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="D48" s="30" t="s">
+      <c r="D48" s="33" t="s">
         <v>42</v>
       </c>
       <c r="E48" s="1">
@@ -2394,7 +2424,7 @@
         <v>92</v>
       </c>
       <c r="C49" s="29"/>
-      <c r="D49" s="30"/>
+      <c r="D49" s="33"/>
       <c r="E49" s="1">
         <v>0.5</v>
       </c>
@@ -2419,7 +2449,7 @@
         <v>93</v>
       </c>
       <c r="C50" s="29"/>
-      <c r="D50" s="30"/>
+      <c r="D50" s="33"/>
       <c r="E50" s="1">
         <v>1</v>
       </c>
@@ -2444,7 +2474,7 @@
         <v>94</v>
       </c>
       <c r="C51" s="29"/>
-      <c r="D51" s="30"/>
+      <c r="D51" s="33"/>
       <c r="E51" s="1">
         <v>0.75</v>
       </c>
@@ -2469,7 +2499,7 @@
         <v>95</v>
       </c>
       <c r="C52" s="29"/>
-      <c r="D52" s="30"/>
+      <c r="D52" s="33"/>
       <c r="E52" s="18" t="s">
         <v>102</v>
       </c>
@@ -2494,10 +2524,10 @@
       <c r="B54" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="C54" s="28" t="s">
+      <c r="C54" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="D54" s="31" t="s">
+      <c r="D54" s="36" t="s">
         <v>43</v>
       </c>
       <c r="E54" s="18" t="s">
@@ -2523,8 +2553,8 @@
       <c r="B55" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C55" s="28"/>
-      <c r="D55" s="30"/>
+      <c r="C55" s="34"/>
+      <c r="D55" s="33"/>
       <c r="E55" s="18" t="s">
         <v>104</v>
       </c>
@@ -2548,8 +2578,8 @@
       <c r="B56" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C56" s="28"/>
-      <c r="D56" s="30"/>
+      <c r="C56" s="34"/>
+      <c r="D56" s="33"/>
       <c r="E56" s="27" t="s">
         <v>121</v>
       </c>
@@ -2573,8 +2603,8 @@
       <c r="B57" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C57" s="28"/>
-      <c r="D57" s="30"/>
+      <c r="C57" s="34"/>
+      <c r="D57" s="33"/>
       <c r="E57" s="27" t="s">
         <v>123</v>
       </c>
@@ -2598,8 +2628,8 @@
       <c r="B58" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="C58" s="28"/>
-      <c r="D58" s="30"/>
+      <c r="C58" s="34"/>
+      <c r="D58" s="33"/>
       <c r="E58" s="18" t="s">
         <v>105</v>
       </c>
@@ -2623,8 +2653,8 @@
       <c r="B59" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C59" s="28"/>
-      <c r="D59" s="30"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="33"/>
       <c r="E59" s="18" t="s">
         <v>106</v>
       </c>
@@ -2666,14 +2696,11 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C9:C14"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="A8:XFD8"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="D9:D14"/>
+    <mergeCell ref="C48:C52"/>
+    <mergeCell ref="D48:D52"/>
+    <mergeCell ref="C54:C59"/>
+    <mergeCell ref="D54:D59"/>
+    <mergeCell ref="A53:XFD53"/>
     <mergeCell ref="C42:C46"/>
     <mergeCell ref="D42:D46"/>
     <mergeCell ref="A39:XFD39"/>
@@ -2685,13 +2712,16 @@
     <mergeCell ref="D27:D36"/>
     <mergeCell ref="D16:D25"/>
     <mergeCell ref="C16:C25"/>
-    <mergeCell ref="C48:C52"/>
-    <mergeCell ref="D48:D52"/>
-    <mergeCell ref="C54:C59"/>
-    <mergeCell ref="D54:D59"/>
-    <mergeCell ref="A53:XFD53"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="A8:XFD8"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="D9:D14"/>
   </mergeCells>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E36" r:id="rId1" xr:uid="{06DC9311-2D25-46B2-8DF2-1A11B71FA734}"/>
   </hyperlinks>

</xml_diff>